<commit_message>
Agenda.xlsx set to "copy to output", should fix 500 error
</commit_message>
<xml_diff>
--- a/zn1Web/Files/Agenda.xlsx
+++ b/zn1Web/Files/Agenda.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Data</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Kowalski Adam</t>
-  </si>
-  <si>
-    <t>Opowieści z Narnii</t>
   </si>
   <si>
     <t>Tytuł</t>
@@ -89,6 +86,21 @@
   </si>
   <si>
     <t>Opowieści z Narnii9</t>
+  </si>
+  <si>
+    <t>Ascos</t>
+  </si>
+  <si>
+    <t>Maciaszczyk Jan</t>
+  </si>
+  <si>
+    <t>Kaizen</t>
+  </si>
+  <si>
+    <t>Kaizen jest praktyką ciągłego doskonalenia. Został wprowadzony i opisany w 1986 przez Masaaki Imai w książce Kaizen: Klucz do sukcesu konkurencyjnego Japonii. Dzisiaj Kaizen jest rozpoznawany na całym świecie jako ważny filar długofalowej strategii konkurencyjnej organizacji.</t>
+  </si>
+  <si>
+    <t>Ofjejknfewmkjfbjwbści z Narnii</t>
   </si>
 </sst>
 </file>
@@ -141,10 +153,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -459,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C35ADFD-B471-4976-BB71-BD65E7C9C264}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -499,14 +511,14 @@
       <c r="B2" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -519,11 +531,11 @@
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,11 +548,11 @@
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -553,11 +565,11 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -570,16 +582,16 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43446</v>
+        <v>43111</v>
       </c>
       <c r="B7" s="2">
         <v>0.75</v>
@@ -587,11 +599,11 @@
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>16</v>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -604,11 +616,11 @@
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -621,11 +633,11 @@
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -638,11 +650,11 @@
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>16</v>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -655,11 +667,28 @@
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>16</v>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42858</v>
+      </c>
+      <c r="B12" s="2">
+        <v>12.125</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change from interop excel to npoi
</commit_message>
<xml_diff>
--- a/zn1Web/Files/Agenda.xlsx
+++ b/zn1Web/Files/Agenda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4470" xr2:uid="{29F12050-75FA-45C2-98A1-8931A38402EC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="4470" xr2:uid="{29F12050-75FA-45C2-98A1-8931A38402EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>